<commit_message>
adding codeMaker work for MILP
</commit_message>
<xml_diff>
--- a/VTOL/milpFormulation/Book1.xlsx
+++ b/VTOL/milpFormulation/Book1.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="150">
   <si>
     <t>ID</t>
   </si>
@@ -473,6 +473,12 @@
   <si>
     <t>3af2-&gt;3bf1 + 3bf2-&gt;3af1 + 3am2-&gt;3bm1 + 3bm2-&gt;3am1 == 1</t>
   </si>
+  <si>
+    <t>m.setObjective(var1am21am1 + var1af11am1 + var1af21am1 + var1ag11am1 + var1ag21am1 + var1bm11am1 + var1bm21am1 + var1bf11am1 + var1bf21am1 + var1bg11am1 + var1bg21am1 + var2am11am1 + var2am21am1 + var2af11am1 + var2af21am1 + var2ag11am1 + var2ag21am1 + var2bm11am1 + var2bm21am1 + var2bf11am1 + var2bf21am1 + var2bg11am1 + var2bg21am1 + var3am11am1 + var3am21am1 + var3af11am1 + var3af21am1 + var3ag11am1 + var3ag21am1 + var3bm11am1 + var3bm21am1 + var3bf11am1 + var3bf21am1 + var3bg11am1 + var3bg21am1 + , GRB.MINIMIZE)</t>
+  </si>
+  <si>
+    <t>m.setObjective(var0am00am1 + var0am00af0 + var0am00af1 + var0am00ag0 + var0am00ag1 + var0am00bm0 + var0am00bm1 + var0am00bf0 + var0am00bf1 + var0am00bg0 + var0am00bg1 + var0am01am0 + var0am01am1 + var0am01af0 + var0am01af1 + var0am01ag0 + var0am01ag1 + var0am01bm0 + var0am01bm1 + var0am01bf0 + var0am01bf1 + var0am01bg0 + var0am01bg1 + var0am02am0 + var0am02am1 + var0am02af0 + var0am02af1 + var0am02ag0 + var0am02ag1 + var0am02bm0 + var0am02bm1 + var0am02bf0 + var0am02bf1 + var0am02bg0 + var0am02bg1 + var0am10am0 + var0am10af0 + var0am10af1 + var0am10ag0 + var0am10ag1 + var0am10bm0 + var0am10bm1 + var0am10bf0 + var0am10bf1 + var0am10bg0 + var0am10bg1 + var0am11am0 + var0am11am1 + var0am11af0 + var0am11af1 + var0am11ag0 + var0am11ag1 + var0am11bm0 + var0am11bm1 + var0am11bf0 + var0am11bf1 + var0am11bg0 + var0am11bg1 + var0am12am0 + var0am12am1 + var0am12af0 + var0am12af1 + var0am12ag0 + var0am12ag1 + var0am12bm0 + var0am12bm1 + var0am12bf0 + var0am12bf1 + var0am12bg0 + var0am12bg1 + var0af00am0 + var0af00am1 + var0af00af1 + var0af00ag0 + var0af00ag1 + var0af00bm0 + var0af00bm1 + var0af00bf0 + var0af00bf1 + var0af00bg0 + var0af00bg1 + var0af01am0 + var0af01am1 + var0af01af0 + var0af01af1 + var0af01ag0 + var0af01ag1 + var0af01bm0 + var0af01bm1 + var0af01bf0 + var0af01bf1 + var0af01bg0 + var0af01bg1 + var0af02am0 + var0af02am1 + var0af02af0 + var0af02af1 + var0af02ag0 + var0af02ag1 + var0af02bm0 + var0af02bm1 + var0af02bf0 + var0af02bf1 + var0af02bg0 + var0af02bg1 + var0af10am0 + var0af10am1 + var0af10af0 + var0af10ag0 + var0af10ag1 + var0af10bm0 + var0af10bm1 + var0af10bf0 + var0af10bf1 + var0af10bg0 + var0af10bg1 + var0af11am0 + var0af11am1 + var0af11af0 + var0af11af1 + var0af11ag0 + var0af11ag1 + var0af11bm0 + var0af11bm1 + var0af11bf0 + var0af11bf1 + var0af11bg0 + var0af11bg1 + var0af12am0 + var0af12am1 + var0af12af0 + var0af12af1 + var0af12ag0 + var0af12ag1 + var0af12bm0 + var0af12bm1 + var0af12bf0 + var0af12bf1 + var0af12bg0 + var0af12bg1 + var0ag00am0 + var0ag00am1 + var0ag00af0 + var0ag00af1 + var0ag00ag1 + var0ag00bm0 + var0ag00bm1 + var0ag00bf0 + var0ag00bf1 + var0ag00bg0 + var0ag00bg1 + var0ag01am0 + var0ag01am1 + var0ag01af0 + var0ag01af1 + var0ag01ag0 + var0ag01ag1 + var0ag01bm0 + var0ag01bm1 + var0ag01bf0 + var0ag01bf1 + var0ag01bg0 + var0ag01bg1 + var0ag02am0 + var0ag02am1 + var0ag02af0 + var0ag02af1 + var0ag02ag0 + var0ag02ag1 + var0ag02bm0 + var0ag02bm1 + var0ag02bf0 + var0ag02bf1 + var0ag02bg0 + var0ag02bg1 + var0ag10am0 + var0ag10am1 + var0ag10af0 + var0ag10af1 + var0ag10ag0 + var0ag10bm0 + var0ag10bm1 + var0ag10bf0 + var0ag10bf1 + var0ag10bg0 + var0ag10bg1 + var0ag11am0 + var0ag11am1 + var0ag11af0 + var0ag11af1 + var0ag11ag0 + var0ag11ag1 + var0ag11bm0 + var0ag11bm1 + var0ag11bf0 + var0ag11bf1 + var0ag11bg0 + var0ag11bg1 + var0ag12am0 + var0ag12am1 + var0ag12af0 + var0ag12af1 + var0ag12ag0 + var0ag12ag1 + var0ag12bm0 + var0ag12bm1 + var0ag12bf0 + var0ag12bf1 + var0ag12bg0 + var0ag12bg1 + var0bm00am0 + var0bm00am1 + var0bm00af0 + var0bm00af1 + var0bm00ag0 + var0bm00ag1 + var0bm00bm1 + var0bm00bf0 + var0bm00bf1 + var0bm00bg0 + var0bm00bg1 + var0bm01am0 + var0bm01am1 + var0bm01af0 + var0bm01af1 + var0bm01ag0 + var0bm01ag1 + var0bm01bm0 + var0bm01bm1 + var0bm01bf0 + var0bm01bf1 + var0bm01bg0 + var0bm01bg1 + var0bm02am0 + var0bm02am1 + var0bm02af0 + var0bm02af1 + var0bm02ag0 + var0bm02ag1 + var0bm02bm0 + var0bm02bm1 + var0bm02bf0 + var0bm02bf1 + var0bm02bg0 + var0bm02bg1 + var0bm10am0 + var0bm10am1 + var0bm10af0 + var0bm10af1 + var0bm10ag0 + var0bm10ag1 + var0bm10bm0 + var0bm10bf0 + var0bm10bf1 + var0bm10bg0 + var0bm10bg1 + var0bm11am0 + var0bm11am1 + var0bm11af0 + var0bm11af1 + var0bm11ag0 + var0bm11ag1 + var0bm11bm0 + var0bm11bm1 + var0bm11bf0 + var0bm11bf1 + var0bm11bg0 + var0bm11bg1 + var0bm12am0 + var0bm12am1 + var0bm12af0 + var0bm12af1 + var0bm12ag0 + var0bm12ag1 + var0bm12bm0 + var0bm12bm1 + var0bm12bf0 + var0bm12bf1 + var0bm12bg0 + var0bm12bg1 + var0bf00am0 + var0bf00am1 + var0bf00af0 + var0bf00af1 + var0bf00ag0 + var0bf00ag1 + var0bf00bm0 + var0bf00bm1 + var0bf00bf1 + var0bf00bg0 + var0bf00bg1 + var0bf01am0 + var0bf01am1 + var0bf01af0 + var0bf01af1 + var0bf01ag0 + var0bf01ag1 + var0bf01bm0 + var0bf01bm1 + var0bf01bf0 + var0bf01bf1 + var0bf01bg0 + var0bf01bg1 + var0bf02am0 + var0bf02am1 + var0bf02af0 + var0bf02af1 + var0bf02ag0 + var0bf02ag1 + var0bf02bm0 + var0bf02bm1 + var0bf02bf0 + var0bf02bf1 + var0bf02bg0 + var0bf02bg1 + var0bf10am0 + var0bf10am1 + var0bf10af0 + var0bf10af1 + var0bf10ag0 + var0bf10ag1 + var0bf10bm0 + var0bf10bm1 + var0bf10bf0 + var0bf10bg0 + var0bf10bg1 + var0bf11am0 + var0bf11am1 + var0bf11af0 + var0bf11af1 + var0bf11ag0 + var0bf11ag1 + var0bf11bm0 + var0bf11bm1 + var0bf11bf0 + var0bf11bf1 + var0bf11bg0 + var0bf11bg1 + var0bf12am0 + var0bf12am1 + var0bf12af0 + var0bf12af1 + var0bf12ag0 + var0bf12ag1 + var0bf12bm0 + var0bf12bm1 + var0bf12bf0 + var0bf12bf1 + var0bf12bg0 + var0bf12bg1 + var0bg00am0 + var0bg00am1 + var0bg00af0 + var0bg00af1 + var0bg00ag0 + var0bg00ag1 + var0bg00bm0 + var0bg00bm1 + var0bg00bf0 + var0bg00bf1 + var0bg00bg1 + var0bg01am0 + var0bg01am1 + var0bg01af0 + var0bg01af1 + var0bg01ag0 + var0bg01ag1 + var0bg01bm0 + var0bg01bm1 + var0bg01bf0 + var0bg01bf1 + var0bg01bg0 + var0bg01bg1 + var0bg02am0 + var0bg02am1 + var0bg02af0 + var0bg02af1 + var0bg02ag0 + var0bg02ag1 + var0bg02bm0 + var0bg02bm1 + var0bg02bf0 + var0bg02bf1 + var0bg02bg0 + var0bg02bg1 + var0bg10am0 + var0bg10am1 + var0bg10af0 + var0bg10af1 + var0bg10ag0 + var0bg10ag1 + var0bg10bm0 + var0bg10bm1 + var0bg10bf0 + var0bg10bf1 + var0bg10bg0 + var0bg11am0 + var0bg11am1 + var0bg11af0 + var0bg11af1 + var0bg11ag0 + var0bg11ag1 + var0bg11bm0 + var0bg11bm1 + var0bg11bf0 + var0bg11bf1 + var0bg11bg0 + var0bg11bg1 + var0bg12am0 + var0bg12am1 + var0bg12af0 + var0bg12af1 + var0bg12ag0 + var0bg12ag1 + var0bg12bm0 + var0bg12bm1 + var0bg12bf0 + var0bg12bf1 + var0bg12bg0 + var0bg12bg1 + var1am00am0 + var1am00am1 + var1am00af0 + var1am00af1 + var1am00ag0 + var1am00ag1 + var1am00bm0 + var1am00bm1 + var1am00bf0 + var1am00bf1 + var1am00bg0 + var1am00bg1 + var1am01am1 + var1am01af0 + var1am01af1 + var1am01ag0 + var1am01ag1 + var1am01bm0 + var1am01bm1 + var1am01bf0 + var1am01bf1 + var1am01bg0 + var1am01bg1 + var1am02am0 + var1am02am1 + var1am02af0 + var1am02af1 + var1am02ag0 + var1am02ag1 + var1am02bm0 + var1am02bm1 + var1am02bf0 + var1am02bf1 + var1am02bg0 + var1am02bg1 + var1am10am0 + var1am10am1 + var1am10af0 + var1am10af1 + var1am10ag0 + var1am10ag1 + var1am10bm0 + var1am10bm1 + var1am10bf0 + var1am10bf1 + var1am10bg0 + var1am10bg1 + var1am11am0 + var1am11af0 + var1am11af1 + var1am11ag0 + var1am11ag1 + var1am11bm0 + var1am11bm1 + var1am11bf0 + var1am11bf1 + var1am11bg0 + var1am11bg1 + var1am12am0 + var1am12am1 + var1am12af0 + var1am12af1 + var1am12ag0 + var1am12ag1 + var1am12bm0 + var1am12bm1 + var1am12bf0 + var1am12bf1 + var1am12bg0 + var1am12bg1 + var1af00am0 + var1af00am1 + var1af00af0 + var1af00af1 + var1af00ag0 + var1af00ag1 + var1af00bm0 + var1af00bm1 + var1af00bf0 + var1af00bf1 + var1af00bg0 + var1af00bg1 + var1af01am0 + var1af01am1 + var1af01af1 + var1af01ag0 + var1af01ag1 + var1af01bm0 + var1af01bm1 + var1af01bf0 + var1af01bf1 + var1af01bg0 + var1af01bg1 + var1af02am0 + var1af02am1 + var1af02af0 + var1af02af1 + var1af02ag0 + var1af02ag1 + var1af02bm0 + var1af02bm1 + var1af02bf0 + var1af02bf1 + var1af02bg0 + var1af02bg1 + var1af10am0 + var1af10am1 + var1af10af0 + var1af10af1 + var1af10ag0 + var1af10ag1 + var1af10bm0 + var1af10bm1 + var1af10bf0 + var1af10bf1 + var1af10bg0 + var1af10bg1 + var1af11am0 + var1af11am1 + var1af11af0 + var1af11ag0 + var1af11ag1 + var1af11bm0 + var1af11bm1 + var1af11bf0 + var1af11bf1 + var1af11bg0 + var1af11bg1 + var1af12am0 + var1af12am1 + var1af12af0 + var1af12af1 + var1af12ag0 + var1af12ag1 + var1af12bm0 + var1af12bm1 + var1af12bf0 + var1af12bf1 + var1af12bg0 + var1af12bg1 + var1ag00am0 + var1ag00am1 + var1ag00af0 + var1ag00af1 + var1ag00ag0 + var1ag00ag1 + var1ag00bm0 + var1ag00bm1 + var1ag00bf0 + var1ag00bf1 + var1ag00bg0 + var1ag00bg1 + var1ag01am0 + var1ag01am1 + var1ag01af0 + var1ag01af1 + var1ag01ag1 + var1ag01bm0 + var1ag01bm1 + var1ag01bf0 + var1ag01bf1 + var1ag01bg0 + var1ag01bg1 + var1ag02am0 + var1ag02am1 + var1ag02af0 + var1ag02af1 + var1ag02ag0 + var1ag02ag1 + var1ag02bm0 + var1ag02bm1 + var1ag02bf0 + var1ag02bf1 + var1ag02bg0 + var1ag02bg1 + var1ag10am0 + var1ag10am1 + var1ag10af0 + var1ag10af1 + var1ag10ag0 + var1ag10ag1 + var1ag10bm0 + var1ag10bm1 + var1ag10bf0 + var1ag10bf1 + var1ag10bg0 + var1ag10bg1 + var1ag11am0 + var1ag11am1 + var1ag11af0 + var1ag11af1 + var1ag11ag0 + var1ag11bm0 + var1ag11bm1 + var1ag11bf0 + var1ag11bf1 + var1ag11bg0 + var1ag11bg1 + var1ag12am0 + var1ag12am1 + var1ag12af0 + var1ag12af1 + var1ag12ag0 + var1ag12ag1 + var1ag12bm0 + var1ag12bm1 + var1ag12bf0 + var1ag12bf1 + var1ag12bg0 + var1ag12bg1 + var1bm00am0 + var1bm00am1 + var1bm00af0 + var1bm00af1 + var1bm00ag0 + var1bm00ag1 + var1bm00bm0 + var1bm00bm1 + var1bm00bf0 + var1bm00bf1 + var1bm00bg0 + var1bm00bg1 + var1bm01am0 + var1bm01am1 + var1bm01af0 + var1bm01af1 + var1bm01ag0 + var1bm01ag1 + var1bm01bm1 + var1bm01bf0 + var1bm01bf1 + var1bm01bg0 + var1bm01bg1 + var1bm02am0 + var1bm02am1 + var1bm02af0 + var1bm02af1 + var1bm02ag0 + var1bm02ag1 + var1bm02bm0 + var1bm02bm1 + var1bm02bf0 + var1bm02bf1 + var1bm02bg0 + var1bm02bg1 + var1bm10am0 + var1bm10am1 + var1bm10af0 + var1bm10af1 + var1bm10ag0 + var1bm10ag1 + var1bm10bm0 + var1bm10bm1 + var1bm10bf0 + var1bm10bf1 + var1bm10bg0 + var1bm10bg1 + var1bm11am0 + var1bm11am1 + var1bm11af0 + var1bm11af1 + var1bm11ag0 + var1bm11ag1 + var1bm11bm0 + var1bm11bf0 + var1bm11bf1 + var1bm11bg0 + var1bm11bg1 + var1bm12am0 + var1bm12am1 + var1bm12af0 + var1bm12af1 + var1bm12ag0 + var1bm12ag1 + var1bm12bm0 + var1bm12bm1 + var1bm12bf0 + var1bm12bf1 + var1bm12bg0 + var1bm12bg1 + var1bf00am0 + var1bf00am1 + var1bf00af0 + var1bf00af1 + var1bf00ag0 + var1bf00ag1 + var1bf00bm0 + var1bf00bm1 + var1bf00bf0 + var1bf00bf1 + var1bf00bg0 + var1bf00bg1 + var1bf01am0 + var1bf01am1 + var1bf01af0 + var1bf01af1 + var1bf01ag0 + var1bf01ag1 + var1bf01bm0 + var1bf01bm1 + var1bf01bf1 + var1bf01bg0 + var1bf01bg1 + var1bf02am0 + var1bf02am1 + var1bf02af0 + var1bf02af1 + var1bf02ag0 + var1bf02ag1 + var1bf02bm0 + var1bf02bm1 + var1bf02bf0 + var1bf02bf1 + var1bf02bg0 + var1bf02bg1 + var1bf10am0 + var1bf10am1 + var1bf10af0 + var1bf10af1 + var1bf10ag0 + var1bf10ag1 + var1bf10bm0 + var1bf10bm1 + var1bf10bf0 + var1bf10bf1 + var1bf10bg0 + var1bf10bg1 + var1bf11am0 + var1bf11am1 + var1bf11af0 + var1bf11af1 + var1bf11ag0 + var1bf11ag1 + var1bf11bm0 + var1bf11bm1 + var1bf11bf0 + var1bf11bg0 + var1bf11bg1 + var1bf12am0 + var1bf12am1 + var1bf12af0 + var1bf12af1 + var1bf12ag0 + var1bf12ag1 + var1bf12bm0 + var1bf12bm1 + var1bf12bf0 + var1bf12bf1 + var1bf12bg0 + var1bf12bg1 + var1bg00am0 + var1bg00am1 + var1bg00af0 + var1bg00af1 + var1bg00ag0 + var1bg00ag1 + var1bg00bm0 + var1bg00bm1 + var1bg00bf0 + var1bg00bf1 + var1bg00bg0 + var1bg00bg1 + var1bg01am0 + var1bg01am1 + var1bg01af0 + var1bg01af1 + var1bg01ag0 + var1bg01ag1 + var1bg01bm0 + var1bg01bm1 + var1bg01bf0 + var1bg01bf1 + var1bg01bg1 + var1bg02am0 + var1bg02am1 + var1bg02af0 + var1bg02af1 + var1bg02ag0 + var1bg02ag1 + var1bg02bm0 + var1bg02bm1 + var1bg02bf0 + var1bg02bf1 + var1bg02bg0 + var1bg02bg1 + var1bg10am0 + var1bg10am1 + var1bg10af0 + var1bg10af1 + var1bg10ag0 + var1bg10ag1 + var1bg10bm0 + var1bg10bm1 + var1bg10bf0 + var1bg10bf1 + var1bg10bg0 + var1bg10bg1 + var1bg11am0 + var1bg11am1 + var1bg11af0 + var1bg11af1 + var1bg11ag0 + var1bg11ag1 + var1bg11bm0 + var1bg11bm1 + var1bg11bf0 + var1bg11bf1 + var1bg11bg0 + var1bg12am0 + var1bg12am1 + var1bg12af0 + var1bg12af1 + var1bg12ag0 + var1bg12ag1 + var1bg12bm0 + var1bg12bm1 + var1bg12bf0 + var1bg12bf1 + var1bg12bg0 + var1bg12bg1 + var2am00am0 + var2am00am1 + var2am00af0 + var2am00af1 + var2am00ag0 + var2am00ag1 + var2am00bm0 + var2am00bm1 + var2am00bf0 + var2am00bf1 + var2am00bg0 + var2am00bg1 + var2am01am0 + var2am01am1 + var2am01af0 + var2am01af1 + var2am01ag0 + var2am01ag1 + var2am01bm0 + var2am01bm1 + var2am01bf0 + var2am01bf1 + var2am01bg0 + var2am01bg1 + var2am02am1 + var2am02af0 + var2am02af1 + var2am02ag0 + var2am02ag1 + var2am02bm0 + var2am02bm1 + var2am02bf0 + var2am02bf1 + var2am02bg0 + var2am02bg1 + var2am10am0 + var2am10am1 + var2am10af0 + var2am10af1 + var2am10ag0 + var2am10ag1 + var2am10bm0 + var2am10bm1 + var2am10bf0 + var2am10bf1 + var2am10bg0 + var2am10bg1 + var2am11am0 + var2am11am1 + var2am11af0 + var2am11af1 + var2am11ag0 + var2am11ag1 + var2am11bm0 + var2am11bm1 + var2am11bf0 + var2am11bf1 + var2am11bg0 + var2am11bg1 + var2am12am0 + var2am12af0 + var2am12af1 + var2am12ag0 + var2am12ag1 + var2am12bm0 + var2am12bm1 + var2am12bf0 + var2am12bf1 + var2am12bg0 + var2am12bg1 + var2af00am0 + var2af00am1 + var2af00af0 + var2af00af1 + var2af00ag0 + var2af00ag1 + var2af00bm0 + var2af00bm1 + var2af00bf0 + var2af00bf1 + var2af00bg0 + var2af00bg1 + var2af01am0 + var2af01am1 + var2af01af0 + var2af01af1 + var2af01ag0 + var2af01ag1 + var2af01bm0 + var2af01bm1 + var2af01bf0 + var2af01bf1 + var2af01bg0 + var2af01bg1 + var2af02am0 + var2af02am1 + var2af02af1 + var2af02ag0 + var2af02ag1 + var2af02bm0 + var2af02bm1 + var2af02bf0 + var2af02bf1 + var2af02bg0 + var2af02bg1 + var2af10am0 + var2af10am1 + var2af10af0 + var2af10af1 + var2af10ag0 + var2af10ag1 + var2af10bm0 + var2af10bm1 + var2af10bf0 + var2af10bf1 + var2af10bg0 + var2af10bg1 + var2af11am0 + var2af11am1 + var2af11af0 + var2af11af1 + var2af11ag0 + var2af11ag1 + var2af11bm0 + var2af11bm1 + var2af11bf0 + var2af11bf1 + var2af11bg0 + var2af11bg1 + var2af12am0 + var2af12am1 + var2af12af0 + var2af12ag0 + var2af12ag1 + var2af12bm0 + var2af12bm1 + var2af12bf0 + var2af12bf1 + var2af12bg0 + var2af12bg1 + var2ag00am0 + var2ag00am1 + var2ag00af0 + var2ag00af1 + var2ag00ag0 + var2ag00ag1 + var2ag00bm0 + var2ag00bm1 + var2ag00bf0 + var2ag00bf1 + var2ag00bg0 + var2ag00bg1 + var2ag01am0 + var2ag01am1 + var2ag01af0 + var2ag01af1 + var2ag01ag0 + var2ag01ag1 + var2ag01bm0 + var2ag01bm1 + var2ag01bf0 + var2ag01bf1 + var2ag01bg0 + var2ag01bg1 + var2ag02am0 + var2ag02am1 + var2ag02af0 + var2ag02af1 + var2ag02ag1 + var2ag02bm0 + var2ag02bm1 + var2ag02bf0 + var2ag02bf1 + var2ag02bg0 + var2ag02bg1 + var2ag10am0 + var2ag10am1 + var2ag10af0 + var2ag10af1 + var2ag10ag0 + var2ag10ag1 + var2ag10bm0 + var2ag10bm1 + var2ag10bf0 + var2ag10bf1 + var2ag10bg0 + var2ag10bg1 + var2ag11am0 + var2ag11am1 + var2ag11af0 + var2ag11af1 + var2ag11ag0 + var2ag11ag1 + var2ag11bm0 + var2ag11bm1 + var2ag11bf0 + var2ag11bf1 + var2ag11bg0 + var2ag11bg1 + var2ag12am0 + var2ag12am1 + var2ag12af0 + var2ag12af1 + var2ag12ag0 + var2ag12bm0 + var2ag12bm1 + var2ag12bf0 + var2ag12bf1 + var2ag12bg0 + var2ag12bg1 + var2bm00am0 + var2bm00am1 + var2bm00af0 + var2bm00af1 + var2bm00ag0 + var2bm00ag1 + var2bm00bm0 + var2bm00bm1 + var2bm00bf0 + var2bm00bf1 + var2bm00bg0 + var2bm00bg1 + var2bm01am0 + var2bm01am1 + var2bm01af0 + var2bm01af1 + var2bm01ag0 + var2bm01ag1 + var2bm01bm0 + var2bm01bm1 + var2bm01bf0 + var2bm01bf1 + var2bm01bg0 + var2bm01bg1 + var2bm02am0 + var2bm02am1 + var2bm02af0 + var2bm02af1 + var2bm02ag0 + var2bm02ag1 + var2bm02bm1 + var2bm02bf0 + var2bm02bf1 + var2bm02bg0 + var2bm02bg1 + var2bm10am0 + var2bm10am1 + var2bm10af0 + var2bm10af1 + var2bm10ag0 + var2bm10ag1 + var2bm10bm0 + var2bm10bm1 + var2bm10bf0 + var2bm10bf1 + var2bm10bg0 + var2bm10bg1 + var2bm11am0 + var2bm11am1 + var2bm11af0 + var2bm11af1 + var2bm11ag0 + var2bm11ag1 + var2bm11bm0 + var2bm11bm1 + var2bm11bf0 + var2bm11bf1 + var2bm11bg0 + var2bm11bg1 + var2bm12am0 + var2bm12am1 + var2bm12af0 + var2bm12af1 + var2bm12ag0 + var2bm12ag1 + var2bm12bm0 + var2bm12bf0 + var2bm12bf1 + var2bm12bg0 + var2bm12bg1 + var2bf00am0 + var2bf00am1 + var2bf00af0 + var2bf00af1 + var2bf00ag0 + var2bf00ag1 + var2bf00bm0 + var2bf00bm1 + var2bf00bf0 + var2bf00bf1 + var2bf00bg0 + var2bf00bg1 + var2bf01am0 + var2bf01am1 + var2bf01af0 + var2bf01af1 + var2bf01ag0 + var2bf01ag1 + var2bf01bm0 + var2bf01bm1 + var2bf01bf0 + var2bf01bf1 + var2bf01bg0 + var2bf01bg1 + var2bf02am0 + var2bf02am1 + var2bf02af0 + var2bf02af1 + var2bf02ag0 + var2bf02ag1 + var2bf02bm0 + var2bf02bm1 + var2bf02bf1 + var2bf02bg0 + var2bf02bg1 + var2bf10am0 + var2bf10am1 + var2bf10af0 + var2bf10af1 + var2bf10ag0 + var2bf10ag1 + var2bf10bm0 + var2bf10bm1 + var2bf10bf0 + var2bf10bf1 + var2bf10bg0 + var2bf10bg1 + var2bf11am0 + var2bf11am1 + var2bf11af0 + var2bf11af1 + var2bf11ag0 + var2bf11ag1 + var2bf11bm0 + var2bf11bm1 + var2bf11bf0 + var2bf11bf1 + var2bf11bg0 + var2bf11bg1 + var2bf12am0 + var2bf12am1 + var2bf12af0 + var2bf12af1 + var2bf12ag0 + var2bf12ag1 + var2bf12bm0 + var2bf12bm1 + var2bf12bf0 + var2bf12bg0 + var2bf12bg1 + var2bg00am0 + var2bg00am1 + var2bg00af0 + var2bg00af1 + var2bg00ag0 + var2bg00ag1 + var2bg00bm0 + var2bg00bm1 + var2bg00bf0 + var2bg00bf1 + var2bg00bg0 + var2bg00bg1 + var2bg01am0 + var2bg01am1 + var2bg01af0 + var2bg01af1 + var2bg01ag0 + var2bg01ag1 + var2bg01bm0 + var2bg01bm1 + var2bg01bf0 + var2bg01bf1 + var2bg01bg0 + var2bg01bg1 + var2bg02am0 + var2bg02am1 + var2bg02af0 + var2bg02af1 + var2bg02ag0 + var2bg02ag1 + var2bg02bm0 + var2bg02bm1 + var2bg02bf0 + var2bg02bf1 + var2bg02bg1 + var2bg10am0 + var2bg10am1 + var2bg10af0 + var2bg10af1 + var2bg10ag0 + var2bg10ag1 + var2bg10bm0 + var2bg10bm1 + var2bg10bf0 + var2bg10bf1 + var2bg10bg0 + var2bg10bg1 + var2bg11am0 + var2bg11am1 + var2bg11af0 + var2bg11af1 + var2bg11ag0 + var2bg11ag1 + var2bg11bm0 + var2bg11bm1 + var2bg11bf0 + var2bg11bf1 + var2bg11bg0 + var2bg11bg1 + var2bg12am0 + var2bg12am1 + var2bg12af0 + var2bg12af1 + var2bg12ag0 + var2bg12ag1 + var2bg12bm0 + var2bg12bm1 + var2bg12bf0 + var2bg12bf1 + var2bg12bg0, GRB.MINIMIZE)</t>
+  </si>
 </sst>
 </file>
 
@@ -5604,10 +5610,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CUZ12"/>
+  <dimension ref="A1:CUZ14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67974,6 +67980,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="13" spans="1:2600" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2600" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>